<commit_message>
Few more mantatory field was created
</commit_message>
<xml_diff>
--- a/public/files/Participant_Bulk_Import_Excel_Format.xlsx
+++ b/public/files/Participant_Bulk_Import_Excel_Format.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t xml:space="preserve">S.No.</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Participant ID</t>
   </si>
   <si>
+    <t xml:space="preserve">Individual Participant</t>
+  </si>
+  <si>
     <t xml:space="preserve">Participant First Name</t>
   </si>
   <si>
@@ -73,6 +76,12 @@
     <t xml:space="preserve">Additional Email ID</t>
   </si>
   <si>
+    <t xml:space="preserve">S12452</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
     <t xml:space="preserve">Siva</t>
   </si>
   <si>
@@ -94,52 +103,61 @@
     <t xml:space="preserve">ZZZZ</t>
   </si>
   <si>
+    <t xml:space="preserve">ATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test@check.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xxx@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S78963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mathi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check@test.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yyy@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S36254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vivek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krishnan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GHI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KLM</t>
+  </si>
+  <si>
     <t xml:space="preserve">IND</t>
   </si>
   <si>
-    <t xml:space="preserve">check@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xxx@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mathi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HIJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test@gmmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yyy@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vivek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Krishnan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GHI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KLM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">private@admin.com</t>
+    <t xml:space="preserve">want@test.com</t>
   </si>
   <si>
     <t xml:space="preserve">zzz@gmail.com</t>
@@ -152,7 +170,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -178,6 +196,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE181E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -232,7 +257,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -245,12 +270,20 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -262,6 +295,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -270,47 +363,47 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="3.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="10.49"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -325,10 +418,10 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -340,190 +433,195 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="n">
-        <v>9512368740</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="I2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="5" t="n">
         <v>654123</v>
       </c>
-      <c r="L2" s="4" t="n">
+      <c r="M2" s="5" t="n">
         <v>12.4578</v>
       </c>
-      <c r="M2" s="4" t="n">
+      <c r="N2" s="5" t="n">
         <v>56.1278</v>
       </c>
-      <c r="N2" s="4" t="n">
-        <v>98745863210</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="4" t="n">
+      <c r="O2" s="5" t="n">
+        <v>9511599513</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="5" t="n">
         <v>12345</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>26</v>
+      <c r="R2" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="n">
-        <v>9512364879</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="4" t="n">
+      <c r="E3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="5" t="n">
         <v>654987</v>
       </c>
-      <c r="L3" s="4" t="n">
+      <c r="M3" s="5" t="n">
         <v>12.3698</v>
       </c>
-      <c r="M3" s="4" t="n">
+      <c r="N3" s="5" t="n">
         <v>56.1473</v>
       </c>
-      <c r="N3" s="4" t="n">
-        <v>98451268920</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="4" t="n">
+      <c r="O3" s="5" t="n">
+        <v>6544566549</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="5" t="n">
         <v>12345</v>
       </c>
-      <c r="Q3" s="4" t="s">
-        <v>33</v>
+      <c r="R3" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="n">
-        <v>789</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="4" t="n">
+      <c r="C4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="5" t="n">
         <v>654159</v>
       </c>
-      <c r="L4" s="4" t="n">
+      <c r="M4" s="5" t="n">
         <v>12.4578</v>
       </c>
-      <c r="M4" s="4" t="n">
+      <c r="N4" s="5" t="n">
         <v>56.3928</v>
       </c>
-      <c r="N4" s="4" t="n">
-        <v>951789</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="4" t="n">
+      <c r="O4" s="5" t="n">
+        <v>8522588521</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="5" t="n">
         <v>12345</v>
       </c>
-      <c r="Q4" s="4" t="s">
-        <v>40</v>
+      <c r="R4" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" display="check@gmail.com"/>
-    <hyperlink ref="Q2" r:id="rId2" display="xxx@gmail.com"/>
-    <hyperlink ref="O3" r:id="rId3" display="test@gmmail.com"/>
-    <hyperlink ref="Q3" r:id="rId4" display="yyy@gmail.com"/>
-    <hyperlink ref="O4" r:id="rId5" display="private@admin.com"/>
-    <hyperlink ref="Q4" r:id="rId6" display="zzz@gmail.com"/>
+    <hyperlink ref="P2" r:id="rId1" display="test@check.com"/>
+    <hyperlink ref="R2" r:id="rId2" display="xxx@gmail.com"/>
+    <hyperlink ref="P3" r:id="rId3" display="check@test.com"/>
+    <hyperlink ref="R3" r:id="rId4" display="yyy@gmail.com"/>
+    <hyperlink ref="P4" r:id="rId5" display="want@test.com"/>
+    <hyperlink ref="R4" r:id="rId6" display="zzz@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added PhpSpreadsheet Library and changed the Participant Bulk Import to use PhpSpreadsheet
</commit_message>
<xml_diff>
--- a/public/files/Participant_Bulk_Import_Excel_Format.xlsx
+++ b/public/files/Participant_Bulk_Import_Excel_Format.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitdugar/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/ept/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDDA8DA9-E9B9-6A4B-9D74-361DFA10094B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585F90E0-32FE-CA47-A0AC-EA415930D806}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Participant LIST" sheetId="1" r:id="rId1"/>
+    <sheet name="Participant List" sheetId="1" r:id="rId1"/>
     <sheet name="Country List" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="796">
   <si>
     <t>S.No.</t>
   </si>
@@ -2408,17 +2408,17 @@
     <t>nrl@example.org</t>
   </si>
   <si>
+    <t>example@gmail.com</t>
+  </si>
+  <si>
+    <t>example2@gmail.com</t>
+  </si>
+  <si>
+    <t>example99@gmail.com</t>
+  </si>
+  <si>
     <t>Password
-(if left blank, the default password is ept@)(*&amp;^</t>
-  </si>
-  <si>
-    <t>example@gmail.com</t>
-  </si>
-  <si>
-    <t>example2@gmail.com</t>
-  </si>
-  <si>
-    <t>example99@gmail.com</t>
+- if left blank, the default password is ept1@)(*&amp;^</t>
   </si>
 </sst>
 </file>
@@ -2891,8 +2891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2918,7 +2918,7 @@
     <col min="19" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>12</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>13</v>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="Q2" s="5"/>
       <c r="R2" s="10" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -3055,7 +3055,9 @@
       <c r="J3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="K3" s="5"/>
+      <c r="K3" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="L3" s="5">
         <v>654987</v>
       </c>
@@ -3073,7 +3075,7 @@
       </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -3125,7 +3127,7 @@
       </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes in Bulk Import format
</commit_message>
<xml_diff>
--- a/public/files/Participant_Bulk_Import_Excel_Format.xlsx
+++ b/public/files/Participant_Bulk_Import_Excel_Format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitdugar/Sites/localhost/ept/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DACFFC-4780-214A-82DB-8175EF119641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518C2739-4F5D-8D4E-A7D0-70D8A08C49E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="797">
   <si>
     <t>S.No.</t>
   </si>
@@ -2422,21 +2422,6 @@
   </si>
   <si>
     <t>District/County</t>
-  </si>
-  <si>
-    <t>SITE01-HTC-01</t>
-  </si>
-  <si>
-    <t>SITE01-HTC-02</t>
-  </si>
-  <si>
-    <t>Amitabh</t>
-  </si>
-  <si>
-    <t>SITE01-HTC-03</t>
-  </si>
-  <si>
-    <t>National Lab</t>
   </si>
 </sst>
 </file>
@@ -2904,11 +2889,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3149,45 +3132,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>797</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>798</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>800</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>801</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Country List'!$B$2:$B$250</xm:f>

</xml_diff>

<commit_message>
Minor change in Participant Bulk Import Excel
</commit_message>
<xml_diff>
--- a/public/files/Participant_Bulk_Import_Excel_Format.xlsx
+++ b/public/files/Participant_Bulk_Import_Excel_Format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitdugar/Sites/localhost/ept/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518C2739-4F5D-8D4E-A7D0-70D8A08C49E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2D673E-E674-F647-923F-CC38273400AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2891,7 +2891,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>